<commit_message>
elements test change the structure
</commit_message>
<xml_diff>
--- a/src/test/java/TestDataDemoQA.xlsx
+++ b/src/test/java/TestDataDemoQA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="URL" sheetId="1" r:id="rId1"/>
@@ -32,164 +32,164 @@
     <t>homePage</t>
   </si>
   <si>
+    <t xml:space="preserve">elementsPage </t>
+  </si>
+  <si>
+    <t>https://demoqa.com/elements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formsPage </t>
+  </si>
+  <si>
+    <t>https://demoqa.com/forms</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/alertsWindows</t>
+  </si>
+  <si>
+    <t>alertsPage</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/widgets</t>
+  </si>
+  <si>
+    <t>widgetsPage</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/interaction</t>
+  </si>
+  <si>
+    <t>interationPage</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/books</t>
+  </si>
+  <si>
+    <t>bookStorePage</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/text-box</t>
+  </si>
+  <si>
+    <t>TextBoxPage</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Current Address</t>
+  </si>
+  <si>
+    <t>Permanent Address</t>
+  </si>
+  <si>
+    <t>bla.bla1@bla.bla</t>
+  </si>
+  <si>
+    <t>bla bla</t>
+  </si>
+  <si>
+    <t>Blablabla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email </t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>First Name Change</t>
+  </si>
+  <si>
+    <t>Jovana</t>
+  </si>
+  <si>
+    <t>re</t>
+  </si>
+  <si>
+    <t>tr</t>
+  </si>
+  <si>
+    <t>456</t>
+  </si>
+  <si>
+    <t>pop</t>
+  </si>
+  <si>
+    <t>yu</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>586</t>
+  </si>
+  <si>
+    <t>ooo</t>
+  </si>
+  <si>
+    <t>BrokenLink</t>
+  </si>
+  <si>
+    <t>http://the-internet.herokuapp.com/status_codes/500</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/automation-practice-form</t>
+  </si>
+  <si>
+    <t>PracticeForm</t>
+  </si>
+  <si>
+    <t>mobile number</t>
+  </si>
+  <si>
+    <t>1234567891</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/sample</t>
+  </si>
+  <si>
+    <t>newTabAlerts</t>
+  </si>
+  <si>
+    <t>Kontic</t>
+  </si>
+  <si>
     <t>https://demoqa.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elementsPage </t>
-  </si>
-  <si>
-    <t>https://demoqa.com/elements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">formsPage </t>
-  </si>
-  <si>
-    <t>https://demoqa.com/forms</t>
-  </si>
-  <si>
-    <t>https://demoqa.com/alertsWindows</t>
-  </si>
-  <si>
-    <t>alertsPage</t>
-  </si>
-  <si>
-    <t>https://demoqa.com/widgets</t>
-  </si>
-  <si>
-    <t>widgetsPage</t>
-  </si>
-  <si>
-    <t>https://demoqa.com/interaction</t>
-  </si>
-  <si>
-    <t>interationPage</t>
-  </si>
-  <si>
-    <t>https://demoqa.com/books</t>
-  </si>
-  <si>
-    <t>bookStorePage</t>
-  </si>
-  <si>
-    <t>https://demoqa.com/text-box</t>
-  </si>
-  <si>
-    <t>TextBoxPage</t>
-  </si>
-  <si>
-    <t>Full Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Current Address</t>
-  </si>
-  <si>
-    <t>Permanent Address</t>
-  </si>
-  <si>
-    <t>bla.bla1@bla.bla</t>
-  </si>
-  <si>
-    <t>bla bla</t>
-  </si>
-  <si>
-    <t>Blablabla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>AS</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email </t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>Salary</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>First Name Change</t>
-  </si>
-  <si>
-    <t>Jovana</t>
-  </si>
-  <si>
-    <t>re</t>
-  </si>
-  <si>
-    <t>tr</t>
-  </si>
-  <si>
-    <t>456</t>
-  </si>
-  <si>
-    <t>pop</t>
-  </si>
-  <si>
-    <t>yu</t>
-  </si>
-  <si>
-    <t>78</t>
-  </si>
-  <si>
-    <t>586</t>
-  </si>
-  <si>
-    <t>ooo</t>
-  </si>
-  <si>
-    <t>BrokenLink</t>
-  </si>
-  <si>
-    <t>http://the-internet.herokuapp.com/status_codes/500</t>
-  </si>
-  <si>
-    <t>https://demoqa.com/automation-practice-form</t>
-  </si>
-  <si>
-    <t>PracticeForm</t>
-  </si>
-  <si>
-    <t>mobile number</t>
-  </si>
-  <si>
-    <t>1234567891</t>
-  </si>
-  <si>
-    <t>https://demoqa.com/sample</t>
-  </si>
-  <si>
-    <t>newTabAlerts</t>
-  </si>
-  <si>
-    <t>Kontic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +203,15 @@
       <color rgb="FF212529"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,16 +231,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -512,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,93 +538,96 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="B1" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
         <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -632,46 +647,46 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -698,35 +713,35 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>TextBox!$B$2</f>
@@ -743,58 +758,58 @@
     </row>
     <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -809,7 +824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -822,29 +837,29 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
elements text box finished
</commit_message>
<xml_diff>
--- a/src/test/java/TestDataDemoQA.xlsx
+++ b/src/test/java/TestDataDemoQA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="URL" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
   <si>
     <t>homePage</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Blablabla</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -183,6 +180,36 @@
   </si>
   <si>
     <t>https://demoqa.com/</t>
+  </si>
+  <si>
+    <t>invalid email</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>1@</t>
+  </si>
+  <si>
+    <t>a@</t>
+  </si>
+  <si>
+    <t>a@1</t>
+  </si>
+  <si>
+    <t>1@a</t>
+  </si>
+  <si>
+    <t>!1@a.com</t>
+  </si>
+  <si>
+    <t>#a@1.com</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -524,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -539,7 +566,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -600,26 +627,26 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
         <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -633,16 +660,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -653,7 +681,7 @@
         <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -663,8 +691,8 @@
       <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
-        <v>22</v>
+      <c r="C2" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -674,8 +702,8 @@
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
-        <v>22</v>
+      <c r="C3" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -685,13 +713,54 @@
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
-        <v>22</v>
+      <c r="C4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1"/>
+    <hyperlink ref="C6" r:id="rId2"/>
+    <hyperlink ref="C7" r:id="rId3"/>
+    <hyperlink ref="C8" r:id="rId4"/>
+    <hyperlink ref="C9" r:id="rId5"/>
+    <hyperlink ref="C10" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <ignoredErrors>
+    <ignoredError sqref="C3" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -713,35 +782,35 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>TextBox!$B$2</f>
@@ -758,58 +827,58 @@
     </row>
     <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -837,29 +906,29 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tests start from elements page added checking if logo button works added some web table tests
</commit_message>
<xml_diff>
--- a/src/test/java/TestDataDemoQA.xlsx
+++ b/src/test/java/TestDataDemoQA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="URL" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
   <si>
     <t>homePage</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>1nvalid</t>
   </si>
 </sst>
 </file>
@@ -662,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,10 +769,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,7 +783,7 @@
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -793,8 +796,11 @@
       <c r="D1" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -807,8 +813,11 @@
       <c r="D2" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -824,8 +833,11 @@
         <f>TextBox!$B$2</f>
         <v>bla.bla1@bla.bla</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="E3" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -838,8 +850,11 @@
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="E4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -852,8 +867,11 @@
       <c r="D5" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -866,8 +884,11 @@
       <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
@@ -879,6 +900,9 @@
       </c>
       <c r="D7" s="2" t="s">
         <v>32</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small fix and continue on web tables
</commit_message>
<xml_diff>
--- a/src/test/java/TestDataDemoQA.xlsx
+++ b/src/test/java/TestDataDemoQA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="URL" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
   <si>
     <t>homePage</t>
   </si>
@@ -215,9 +215,6 @@
     <t>1nvalid</t>
   </si>
   <si>
-    <t>=TextBox!$B$2</t>
-  </si>
-  <si>
     <t>webTablesPage</t>
   </si>
   <si>
@@ -234,6 +231,12 @@
   </si>
   <si>
     <t>radioButtonPage</t>
+  </si>
+  <si>
+    <t>maxlengthaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaagrg1nvalid</t>
+  </si>
+  <si>
+    <t>123456789123</t>
   </si>
 </sst>
 </file>
@@ -286,12 +289,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -575,7 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -675,18 +679,18 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" t="s">
         <v>63</v>
-      </c>
-      <c r="B12" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -699,10 +703,10 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -719,7 +723,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,7 +748,7 @@
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -811,9 +815,10 @@
     <hyperlink ref="C8" r:id="rId4"/>
     <hyperlink ref="C9" r:id="rId5"/>
     <hyperlink ref="C10" r:id="rId6"/>
+    <hyperlink ref="B2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
   <ignoredErrors>
     <ignoredError sqref="C3" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -822,10 +827,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,10 +838,12 @@
     <col min="1" max="1" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="52" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -852,8 +859,11 @@
       <c r="E1" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -869,27 +879,29 @@
       <c r="E2" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="2" t="str">
-        <f>TextBox!$B$2</f>
-        <v>bla.bla1@bla.bla</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="2" t="str">
-        <f>TextBox!$B$2</f>
-        <v>bla.bla1@bla.bla</v>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="F3"/>
+    </row>
+    <row r="4" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -905,8 +917,11 @@
       <c r="E4" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -922,8 +937,11 @@
       <c r="E5" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="F5" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -939,8 +957,11 @@
       <c r="E6" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="F6" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
finishing web tables and starting buttons
</commit_message>
<xml_diff>
--- a/src/test/java/TestDataDemoQA.xlsx
+++ b/src/test/java/TestDataDemoQA.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="72">
   <si>
     <t>homePage</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>123456789123</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/buttons</t>
+  </si>
+  <si>
+    <t>buttonsPage</t>
   </si>
 </sst>
 </file>
@@ -577,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,6 +705,14 @@
       </c>
       <c r="B14" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>